<commit_message>
fix: Add the localisation of missing data
tags: fix, data

Why:
- There were issues on cities and postal codes

What:
- Update the raw data file
</commit_message>
<xml_diff>
--- a/inst/data-projects-raw/PGV.xlsx
+++ b/inst/data-projects-raw/PGV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\PrävGesVer\1. Projektförderung PGV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margotbrard/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B49E8A-A0BA-4B99-8704-74B075F17FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEDD1D6-6CBB-B841-A899-C00029D94006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="15840" xr2:uid="{6B07E172-3357-4C84-A0A5-2E4027809C22}"/>
+    <workbookView xWindow="17360" yWindow="500" windowWidth="33840" windowHeight="15840" xr2:uid="{6B07E172-3357-4C84-A0A5-2E4027809C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2934" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2936" uniqueCount="728">
   <si>
     <t>Kurztitel</t>
   </si>
@@ -4560,7 +4559,7 @@
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
     <numFmt numFmtId="165" formatCode="_ [$CHF-807]\ * #,##0_ ;_ [$CHF-807]\ * \-#,##0_ ;_ [$CHF-807]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4644,6 +4643,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -4709,7 +4715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -4859,6 +4865,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -5178,10 +5188,10 @@
   <dimension ref="A1:AL69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="19" style="34"/>
     <col min="6" max="6" width="19" style="34"/>
@@ -5193,7 +5203,7 @@
     <col min="39" max="16384" width="19" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -5309,7 +5319,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="2" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>341</v>
       </c>
@@ -5409,7 +5419,7 @@
       <c r="AK2" s="32"/>
       <c r="AL2" s="32"/>
     </row>
-    <row r="3" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
         <v>33</v>
       </c>
@@ -5522,7 +5532,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="4" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="35" t="s">
         <v>8</v>
       </c>
@@ -5556,8 +5566,8 @@
       <c r="K4" s="35" t="s">
         <v>727</v>
       </c>
-      <c r="L4" s="35" t="s">
-        <v>266</v>
+      <c r="L4" s="35">
+        <v>1951</v>
       </c>
       <c r="M4" s="35" t="s">
         <v>309</v>
@@ -5629,7 +5639,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="5" spans="1:38" s="49" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" s="49" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
         <v>389</v>
       </c>
@@ -5743,7 +5753,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="6" spans="1:38" s="49" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" s="49" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
         <v>32</v>
       </c>
@@ -5853,7 +5863,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="7" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
         <v>47</v>
       </c>
@@ -5942,7 +5952,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="8" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="35" t="s">
         <v>11</v>
       </c>
@@ -6055,7 +6065,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="9" spans="1:38" s="49" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" s="49" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="38" t="s">
         <v>386</v>
       </c>
@@ -6169,7 +6179,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="10" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
         <v>46</v>
       </c>
@@ -6258,7 +6268,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="11" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
         <v>42</v>
       </c>
@@ -6371,7 +6381,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="12" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
         <v>39</v>
       </c>
@@ -6481,7 +6491,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="13" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
         <v>34</v>
       </c>
@@ -6591,7 +6601,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="14" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="35" t="s">
         <v>31</v>
       </c>
@@ -6704,7 +6714,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="15" spans="1:38" s="49" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" s="49" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="38" t="s">
         <v>7</v>
       </c>
@@ -6820,7 +6830,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="16" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
         <v>10</v>
       </c>
@@ -6930,7 +6940,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="17" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="35" t="s">
         <v>37</v>
       </c>
@@ -7043,7 +7053,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="18" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="35" t="s">
         <v>38</v>
       </c>
@@ -7150,7 +7160,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="19" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
         <v>36</v>
       </c>
@@ -7263,7 +7273,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="20" spans="1:38" s="49" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" s="49" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>384</v>
       </c>
@@ -7375,7 +7385,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="21" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
         <v>21</v>
       </c>
@@ -7491,7 +7501,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="22" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
         <v>22</v>
       </c>
@@ -7604,7 +7614,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="23" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>48</v>
       </c>
@@ -7638,8 +7648,12 @@
       <c r="K23" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
+      <c r="L23" s="35">
+        <v>1003</v>
+      </c>
+      <c r="M23" s="35" t="s">
+        <v>299</v>
+      </c>
       <c r="N23" s="24"/>
       <c r="O23" s="2" t="s">
         <v>325</v>
@@ -7670,7 +7684,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="24" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -7780,7 +7794,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="25" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>395</v>
       </c>
@@ -7879,7 +7893,7 @@
       <c r="AK25" s="30"/>
       <c r="AL25" s="30"/>
     </row>
-    <row r="26" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -7989,7 +8003,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="27" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>401</v>
       </c>
@@ -8085,7 +8099,7 @@
       <c r="AK27" s="30"/>
       <c r="AL27" s="30"/>
     </row>
-    <row r="28" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>5</v>
       </c>
@@ -8195,7 +8209,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="29" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
@@ -8302,7 +8316,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="30" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>402</v>
       </c>
@@ -8400,7 +8414,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="31" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>392</v>
       </c>
@@ -8490,7 +8504,7 @@
       <c r="AK31" s="30"/>
       <c r="AL31" s="30"/>
     </row>
-    <row r="32" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>4</v>
       </c>
@@ -8600,7 +8614,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="33" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>3</v>
       </c>
@@ -8710,7 +8724,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="34" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -8820,7 +8834,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="35" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>29</v>
       </c>
@@ -8930,7 +8944,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="36" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>30</v>
       </c>
@@ -9034,7 +9048,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="37" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>24</v>
       </c>
@@ -9071,8 +9085,8 @@
       <c r="L37" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="M37" s="2" t="s">
-        <v>305</v>
+      <c r="M37" s="50" t="s">
+        <v>302</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>315</v>
@@ -9144,7 +9158,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="38" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>20</v>
       </c>
@@ -9254,7 +9268,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="39" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>40</v>
       </c>
@@ -9362,7 +9376,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="40" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>381</v>
       </c>
@@ -9466,7 +9480,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="41" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>28</v>
       </c>
@@ -9573,7 +9587,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="42" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>388</v>
       </c>
@@ -9683,7 +9697,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="43" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>27</v>
       </c>
@@ -9799,7 +9813,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="44" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>12</v>
       </c>
@@ -9912,7 +9926,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="45" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>9</v>
       </c>
@@ -10022,7 +10036,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="46" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>377</v>
       </c>
@@ -10126,7 +10140,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="47" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>15</v>
       </c>
@@ -10239,7 +10253,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="48" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>383</v>
       </c>
@@ -10355,7 +10369,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="49" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>23</v>
       </c>
@@ -10462,7 +10476,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="50" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>25</v>
       </c>
@@ -10572,7 +10586,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="51" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>380</v>
       </c>
@@ -10688,7 +10702,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="52" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>35</v>
       </c>
@@ -10804,7 +10818,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="53" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>1</v>
       </c>
@@ -10917,7 +10931,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="54" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>18</v>
       </c>
@@ -11030,7 +11044,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="55" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>17</v>
       </c>
@@ -11140,7 +11154,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="56" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>390</v>
       </c>
@@ -11244,7 +11258,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="57" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>13</v>
       </c>
@@ -11351,7 +11365,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="58" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>387</v>
       </c>
@@ -11464,7 +11478,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="59" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>43</v>
       </c>
@@ -11574,7 +11588,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="60" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>379</v>
       </c>
@@ -11681,7 +11695,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="61" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>14</v>
       </c>
@@ -11794,7 +11808,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="62" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>382</v>
       </c>
@@ -11901,7 +11915,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="63" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>378</v>
       </c>
@@ -12014,7 +12028,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="64" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>26</v>
       </c>
@@ -12124,7 +12138,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="65" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>385</v>
       </c>
@@ -12237,7 +12251,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="66" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>19</v>
       </c>
@@ -12347,7 +12361,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="67" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>41</v>
       </c>
@@ -12463,7 +12477,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="68" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>45</v>
       </c>
@@ -12573,7 +12587,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="69" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:38" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="34" t="s">
         <v>594</v>
       </c>
@@ -12595,6 +12609,12 @@
       <c r="G69" s="11">
         <v>45747</v>
       </c>
+      <c r="L69" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="M69" s="25" t="s">
+        <v>299</v>
+      </c>
       <c r="AI69" s="34" t="s">
         <v>595</v>
       </c>
@@ -12609,7 +12629,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="N1:N69" xr:uid="{E218302B-3DB1-4C63-8F3D-9B67A7D7BAE1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AH68">
     <sortCondition ref="A1:A68"/>
   </sortState>
@@ -12625,16 +12644,16 @@
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="30"/>
-    <col min="3" max="3" width="54.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="66.140625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="30"/>
+    <col min="1" max="1" width="27.5" style="30" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="30"/>
+    <col min="3" max="3" width="54.1640625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="66.1640625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>516</v>
       </c>
@@ -12651,7 +12670,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>519</v>
       </c>
@@ -12668,7 +12687,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
         <v>524</v>
       </c>
@@ -12685,7 +12704,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
         <v>389</v>
       </c>
@@ -12702,7 +12721,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
         <v>32</v>
       </c>
@@ -12719,7 +12738,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>537</v>
       </c>
@@ -12736,7 +12755,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
         <v>469</v>
       </c>
@@ -12753,7 +12772,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
         <v>386</v>
       </c>
@@ -12770,7 +12789,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
         <v>546</v>
       </c>
@@ -12787,7 +12806,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
         <v>550</v>
       </c>
@@ -12804,7 +12823,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
         <v>487</v>
       </c>
@@ -12821,7 +12840,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="30" t="s">
         <v>557</v>
       </c>
@@ -12838,7 +12857,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
         <v>561</v>
       </c>
@@ -12855,7 +12874,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
         <v>7</v>
       </c>
@@ -12872,7 +12891,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="30" t="s">
         <v>565</v>
       </c>
@@ -12889,7 +12908,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
         <v>37</v>
       </c>
@@ -12906,7 +12925,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
         <v>38</v>
       </c>
@@ -12923,7 +12942,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
         <v>36</v>
       </c>
@@ -12940,7 +12959,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
         <v>577</v>
       </c>
@@ -12957,7 +12976,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
         <v>475</v>
       </c>
@@ -12974,7 +12993,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
         <v>22</v>
       </c>
@@ -12991,7 +13010,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>16</v>
       </c>
@@ -13008,7 +13027,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
         <v>6</v>
       </c>
@@ -13025,7 +13044,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="30" t="s">
         <v>5</v>
       </c>
@@ -13042,7 +13061,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
         <v>2</v>
       </c>
@@ -13059,7 +13078,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
         <v>594</v>
       </c>
@@ -13076,7 +13095,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
         <v>4</v>
       </c>
@@ -13093,7 +13112,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="30" t="s">
         <v>3</v>
       </c>
@@ -13110,7 +13129,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
         <v>603</v>
       </c>
@@ -13127,7 +13146,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="30" t="s">
         <v>481</v>
       </c>
@@ -13144,7 +13163,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="30" t="s">
         <v>609</v>
       </c>
@@ -13161,7 +13180,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="s">
         <v>613</v>
       </c>
@@ -13178,7 +13197,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="30" t="s">
         <v>616</v>
       </c>
@@ -13195,7 +13214,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="30" t="s">
         <v>617</v>
       </c>
@@ -13209,7 +13228,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="30" t="s">
         <v>381</v>
       </c>
@@ -13226,7 +13245,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="30" t="s">
         <v>480</v>
       </c>
@@ -13243,7 +13262,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="30" t="s">
         <v>388</v>
       </c>
@@ -13260,7 +13279,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="30" t="s">
         <v>479</v>
       </c>
@@ -13277,7 +13296,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="30" t="s">
         <v>632</v>
       </c>
@@ -13294,7 +13313,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="30" t="s">
         <v>636</v>
       </c>
@@ -13311,7 +13330,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="30" t="s">
         <v>377</v>
       </c>
@@ -13328,7 +13347,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="30" t="s">
         <v>15</v>
       </c>
@@ -13345,7 +13364,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="30" t="s">
         <v>645</v>
       </c>
@@ -13362,7 +13381,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="30" t="s">
         <v>476</v>
       </c>
@@ -13379,7 +13398,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="30" t="s">
         <v>655</v>
       </c>
@@ -13396,7 +13415,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="30" t="s">
         <v>659</v>
       </c>
@@ -13413,7 +13432,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="30" t="s">
         <v>662</v>
       </c>
@@ -13430,7 +13449,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="30" t="s">
         <v>666</v>
       </c>
@@ -13447,7 +13466,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="30" t="s">
         <v>18</v>
       </c>
@@ -13464,7 +13483,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="30" t="s">
         <v>17</v>
       </c>
@@ -13481,7 +13500,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="30" t="s">
         <v>390</v>
       </c>
@@ -13498,7 +13517,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="30" t="s">
         <v>675</v>
       </c>
@@ -13515,7 +13534,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="30" t="s">
         <v>649</v>
       </c>
@@ -13532,7 +13551,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="30" t="s">
         <v>678</v>
       </c>
@@ -13549,7 +13568,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="30" t="s">
         <v>681</v>
       </c>
@@ -13566,7 +13585,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="30" t="s">
         <v>472</v>
       </c>
@@ -13583,7 +13602,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="30" t="s">
         <v>686</v>
       </c>
@@ -13600,7 +13619,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="30" t="s">
         <v>690</v>
       </c>
@@ -13617,7 +13636,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="30" t="s">
         <v>26</v>
       </c>
@@ -13634,7 +13653,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="30" t="s">
         <v>696</v>
       </c>
@@ -13651,7 +13670,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="30" t="s">
         <v>473</v>
       </c>
@@ -13668,7 +13687,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="30" t="s">
         <v>703</v>
       </c>
@@ -13685,7 +13704,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="30" t="s">
         <v>493</v>
       </c>
@@ -13702,7 +13721,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="30" t="s">
         <v>594</v>
       </c>
@@ -13733,27 +13752,27 @@
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="16"/>
-    <col min="4" max="4" width="27.28515625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="30.5" style="16" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="16"/>
+    <col min="4" max="4" width="27.33203125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="16" customWidth="1"/>
     <col min="7" max="8" width="11" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="10.85546875" style="16"/>
+    <col min="9" max="12" width="10.83203125" style="16"/>
     <col min="13" max="13" width="11" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="16"/>
-    <col min="15" max="15" width="25.28515625" style="16" customWidth="1"/>
-    <col min="16" max="16" width="24.5703125" style="16" customWidth="1"/>
-    <col min="17" max="20" width="10.85546875" style="16"/>
-    <col min="21" max="24" width="14.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="10.85546875" style="16"/>
+    <col min="14" max="14" width="10.83203125" style="16"/>
+    <col min="15" max="15" width="25.33203125" style="16" customWidth="1"/>
+    <col min="16" max="16" width="24.5" style="16" customWidth="1"/>
+    <col min="17" max="20" width="10.83203125" style="16"/>
+    <col min="21" max="24" width="14.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="10.83203125" style="16"/>
     <col min="31" max="39" width="11" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" s="23" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -13872,7 +13891,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="23" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" s="23" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>497</v>
       </c>
@@ -13983,7 +14002,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>377</v>
       </c>
@@ -14090,7 +14109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="14.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" ht="14.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>465</v>
       </c>
@@ -14196,7 +14215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
@@ -14298,7 +14317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
@@ -14403,7 +14422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -14508,7 +14527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -14611,7 +14630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -14716,7 +14735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
@@ -14824,7 +14843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>466</v>
       </c>
@@ -14933,7 +14952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>378</v>
       </c>
@@ -15035,7 +15054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>379</v>
       </c>
@@ -15143,7 +15162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>467</v>
       </c>
@@ -15243,7 +15262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>468</v>
       </c>
@@ -15346,7 +15365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>469</v>
       </c>
@@ -15449,7 +15468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>380</v>
       </c>
@@ -15557,7 +15576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>470</v>
       </c>
@@ -15668,7 +15687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>471</v>
       </c>
@@ -15774,7 +15793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>472</v>
       </c>
@@ -15874,7 +15893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>15</v>
       </c>
@@ -15980,7 +15999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>16</v>
       </c>
@@ -16086,7 +16105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>17</v>
       </c>
@@ -16189,7 +16208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>18</v>
       </c>
@@ -16292,7 +16311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>473</v>
       </c>
@@ -16398,7 +16417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>474</v>
       </c>
@@ -16501,7 +16520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>390</v>
       </c>
@@ -16606,7 +16625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>381</v>
       </c>
@@ -16705,7 +16724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>475</v>
       </c>
@@ -16802,7 +16821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>22</v>
       </c>
@@ -16911,7 +16930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>476</v>
       </c>
@@ -17017,7 +17036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>477</v>
       </c>
@@ -17117,7 +17136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>382</v>
       </c>
@@ -17222,7 +17241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
         <v>478</v>
       </c>
@@ -17322,7 +17341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>383</v>
       </c>
@@ -17427,7 +17446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>26</v>
       </c>
@@ -17536,7 +17555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>479</v>
       </c>
@@ -17639,7 +17658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>480</v>
       </c>
@@ -17748,7 +17767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>384</v>
       </c>
@@ -17850,7 +17869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>481</v>
       </c>
@@ -17953,7 +17972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
         <v>482</v>
       </c>
@@ -18056,7 +18075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
         <v>483</v>
       </c>
@@ -18153,7 +18172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>32</v>
       </c>
@@ -18261,7 +18280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>484</v>
       </c>
@@ -18361,7 +18380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
         <v>485</v>
       </c>
@@ -18467,7 +18486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>486</v>
       </c>
@@ -18570,7 +18589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>385</v>
       </c>
@@ -18681,7 +18700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>387</v>
       </c>
@@ -18789,7 +18808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
         <v>386</v>
       </c>
@@ -18897,7 +18916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
         <v>389</v>
       </c>
@@ -19005,7 +19024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
         <v>36</v>
       </c>
@@ -19111,7 +19130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
         <v>37</v>
       </c>
@@ -19217,7 +19236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>38</v>
       </c>
@@ -19323,7 +19342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
         <v>487</v>
       </c>
@@ -19423,7 +19442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>488</v>
       </c>
@@ -19526,7 +19545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
         <v>489</v>
       </c>
@@ -19629,7 +19648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
         <v>490</v>
       </c>
@@ -19738,7 +19757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
         <v>491</v>
       </c>
@@ -19844,7 +19863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
         <v>492</v>
       </c>
@@ -19947,7 +19966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
         <v>493</v>
       </c>
@@ -20050,7 +20069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
         <v>388</v>
       </c>
@@ -20155,7 +20174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
         <v>494</v>
       </c>
@@ -20258,7 +20277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
         <v>495</v>
       </c>
@@ -20358,7 +20377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
         <v>48</v>
       </c>
@@ -20415,7 +20434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1048576" spans="13:39" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1048576" spans="13:39" hidden="1" x14ac:dyDescent="0.2">
       <c r="M1048576" s="16">
         <f>SUM(M3:M1048575)</f>
         <v>3110</v>

</xml_diff>

<commit_message>
data: Fix missng values and typos in raw data
tags: data, fix

Why:
- Some cities were missing
- Some ZIP codes were missing
- Some ZIP codes were not correct

What:
- Modify the raw Excel file
</commit_message>
<xml_diff>
--- a/inst/data-projects-raw/PGV.xlsx
+++ b/inst/data-projects-raw/PGV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margotbrard/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6289E50-924B-894C-ADBB-B4F930F98335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9ECDC8-925C-384D-B499-C495FD03B6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38640" windowHeight="20120" xr2:uid="{6B07E172-3357-4C84-A0A5-2E4027809C22}"/>
+    <workbookView xWindow="3620" yWindow="500" windowWidth="20800" windowHeight="20120" xr2:uid="{6B07E172-3357-4C84-A0A5-2E4027809C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3188" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3190" uniqueCount="926">
   <si>
     <t>Kurztitel</t>
   </si>
@@ -5176,7 +5176,7 @@
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
     <numFmt numFmtId="165" formatCode="_ [$CHF-807]\ * #,##0_ ;_ [$CHF-807]\ * \-#,##0_ ;_ [$CHF-807]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5266,6 +5266,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -5343,7 +5350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -5463,6 +5470,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5779,8 +5787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E218302B-3DB1-4C63-8F3D-9B67A7D7BAE1}">
   <dimension ref="A1:AP69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL5" sqref="AL5"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6183,8 +6191,8 @@
       <c r="K4" s="27" t="s">
         <v>727</v>
       </c>
-      <c r="L4" s="27" t="s">
-        <v>266</v>
+      <c r="L4" s="45">
+        <v>1951</v>
       </c>
       <c r="M4" s="27" t="s">
         <v>309</v>
@@ -8474,8 +8482,12 @@
       <c r="K23" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
+      <c r="L23" s="39">
+        <v>1003</v>
+      </c>
+      <c r="M23" s="39" t="s">
+        <v>299</v>
+      </c>
       <c r="N23" s="39"/>
       <c r="O23" s="2" t="s">
         <v>325</v>
@@ -10021,8 +10033,8 @@
       <c r="L37" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="M37" s="2" t="s">
-        <v>305</v>
+      <c r="M37" s="27" t="s">
+        <v>302</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>315</v>
@@ -13927,6 +13939,12 @@
       </c>
       <c r="G69" s="9">
         <v>45747</v>
+      </c>
+      <c r="L69" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="M69" s="22" t="s">
+        <v>299</v>
       </c>
       <c r="Z69"/>
       <c r="AA69"/>
@@ -13960,7 +13978,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="N1:N69" xr:uid="{E218302B-3DB1-4C63-8F3D-9B67A7D7BAE1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AH68">
     <sortCondition ref="A1:A68"/>
   </sortState>

</xml_diff>